<commit_message>
south, yuktahar mistakes rectified
</commit_message>
<xml_diff>
--- a/excel_menu/southmess.xlsx
+++ b/excel_menu/southmess.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="149">
   <si>
     <t xml:space="preserve">Meal</t>
   </si>
@@ -58,7 +58,7 @@
     <t xml:space="preserve">Upma</t>
   </si>
   <si>
-    <t xml:space="preserve">Poori</t>
+    <t xml:space="preserve">Poha</t>
   </si>
   <si>
     <t xml:space="preserve">Dalia</t>
@@ -166,7 +166,7 @@
     <t xml:space="preserve">Dosakaya</t>
   </si>
   <si>
-    <t xml:space="preserve">Kakarakaya/Brinjal onions</t>
+    <t xml:space="preserve">Kakarakaya</t>
   </si>
   <si>
     <t xml:space="preserve">Aloo fry</t>
@@ -266,6 +266,9 @@
   </si>
   <si>
     <t xml:space="preserve">Pulao</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tomato Rice</t>
   </si>
   <si>
     <t xml:space="preserve">Paneer / Veg Dum Biryani</t>
@@ -342,9 +345,6 @@
     <t xml:space="preserve">Dinner</t>
   </si>
   <si>
-    <t xml:space="preserve">Aloo 65</t>
-  </si>
-  <si>
     <t xml:space="preserve">Dondakaya curry/ beetroot</t>
   </si>
   <si>
@@ -445,9 +445,6 @@
   </si>
   <si>
     <t xml:space="preserve">Spl Rice</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tomato Rice</t>
   </si>
   <si>
     <t xml:space="preserve">Dadhojanam</t>
@@ -895,11 +892,11 @@
   </sheetPr>
   <dimension ref="A1:I30"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A18" activeCellId="0" sqref="A18"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A3" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C23" activeCellId="0" sqref="C23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.70703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="12.15"/>
@@ -1239,51 +1236,53 @@
       <c r="G13" s="16" t="s">
         <v>81</v>
       </c>
-      <c r="H13" s="17"/>
+      <c r="H13" s="19" t="s">
+        <v>82</v>
+      </c>
       <c r="I13" s="20" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="14"/>
       <c r="B14" s="15" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C14" s="16"/>
       <c r="D14" s="17"/>
       <c r="E14" s="17"/>
       <c r="F14" s="16"/>
       <c r="G14" s="16" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="H14" s="16" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="I14" s="21"/>
     </row>
     <row r="15" s="12" customFormat="true" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="14"/>
       <c r="B15" s="15" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C15" s="16" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="D15" s="16"/>
       <c r="E15" s="16" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="F15" s="16" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="G15" s="16" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="H15" s="16" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="I15" s="19" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="28.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1294,15 +1293,15 @@
       <c r="C16" s="16"/>
       <c r="D16" s="16"/>
       <c r="E16" s="16" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="F16" s="16" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="G16" s="17"/>
       <c r="H16" s="17"/>
       <c r="I16" s="19" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row r="17" s="12" customFormat="true" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1311,54 +1310,54 @@
         <v>41</v>
       </c>
       <c r="C17" s="18" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D17" s="18" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="E17" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="F17" s="18" t="s">
         <v>94</v>
       </c>
-      <c r="F17" s="18" t="s">
-        <v>93</v>
-      </c>
       <c r="G17" s="18" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="H17" s="18" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="I17" s="18" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="22" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B18" s="23" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C18" s="24" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="D18" s="24" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="E18" s="24" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="F18" s="24" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="G18" s="24" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="H18" s="24" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="I18" s="25" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="19" s="12" customFormat="true" ht="28.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1367,37 +1366,35 @@
         <v>26</v>
       </c>
       <c r="C19" s="27" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D19" s="27" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="E19" s="27" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="F19" s="27" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="G19" s="27" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="H19" s="27" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="I19" s="27" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="28" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B20" s="29" t="s">
         <v>44</v>
       </c>
-      <c r="C20" s="30" t="s">
-        <v>106</v>
-      </c>
+      <c r="C20" s="30"/>
       <c r="D20" s="31"/>
       <c r="E20" s="31"/>
       <c r="F20" s="30" t="s">
@@ -1558,7 +1555,7 @@
       </c>
       <c r="C27" s="31"/>
       <c r="D27" s="30" t="s">
-        <v>141</v>
+        <v>82</v>
       </c>
       <c r="E27" s="31"/>
       <c r="F27" s="31"/>
@@ -1567,47 +1564,47 @@
         <v>78</v>
       </c>
       <c r="I27" s="32" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="28"/>
       <c r="B28" s="29" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C28" s="31"/>
       <c r="D28" s="30" t="s">
+        <v>142</v>
+      </c>
+      <c r="E28" s="30" t="s">
         <v>143</v>
-      </c>
-      <c r="E28" s="30" t="s">
-        <v>144</v>
       </c>
       <c r="F28" s="31"/>
       <c r="G28" s="31"/>
       <c r="H28" s="30"/>
       <c r="I28" s="32" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="28"/>
       <c r="B29" s="29" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C29" s="30" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D29" s="31"/>
       <c r="E29" s="31"/>
       <c r="F29" s="30" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="G29" s="30" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="H29" s="31"/>
       <c r="I29" s="32" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="30" s="12" customFormat="true" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1616,25 +1613,25 @@
         <v>41</v>
       </c>
       <c r="C30" s="34" t="s">
+        <v>147</v>
+      </c>
+      <c r="D30" s="35" t="s">
+        <v>147</v>
+      </c>
+      <c r="E30" s="34" t="s">
+        <v>147</v>
+      </c>
+      <c r="F30" s="34" t="s">
+        <v>147</v>
+      </c>
+      <c r="G30" s="35" t="s">
+        <v>147</v>
+      </c>
+      <c r="H30" s="35" t="s">
+        <v>147</v>
+      </c>
+      <c r="I30" s="36" t="s">
         <v>148</v>
-      </c>
-      <c r="D30" s="35" t="s">
-        <v>148</v>
-      </c>
-      <c r="E30" s="34" t="s">
-        <v>148</v>
-      </c>
-      <c r="F30" s="34" t="s">
-        <v>148</v>
-      </c>
-      <c r="G30" s="35" t="s">
-        <v>148</v>
-      </c>
-      <c r="H30" s="35" t="s">
-        <v>148</v>
-      </c>
-      <c r="I30" s="36" t="s">
-        <v>149</v>
       </c>
     </row>
   </sheetData>

</xml_diff>